<commit_message>
Added Gnatt Chart and some other fixes
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531499\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531499\Desktop\GDP1\project-charter-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECD1D23-8FEB-4537-9E1C-EB8A0747E078}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D3914-6401-4540-9B16-21FA1FF3A42A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{8B16F639-4901-4C49-AF1F-A7EDAC1069E8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>DATE</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Student Union</t>
+  </si>
+  <si>
+    <t>2:00PM</t>
   </si>
 </sst>
 </file>
@@ -109,10 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77472347-4511-4D01-BB25-758FE3AE7E08}">
   <dimension ref="A5:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +447,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -507,7 +513,15 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>43381</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>